<commit_message>
Use SIC classification from EDGAR records
</commit_message>
<xml_diff>
--- a/data/weights_sp500_feb_7_2023.xlsx
+++ b/data/weights_sp500_feb_7_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20204972\Documents\evidential-hmm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE75300-679C-470D-B4B2-56172C249E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B26011-4D89-42F2-B781-CB3478D9565C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FB1E3C0E-653D-4DA7-A093-4271DA0134D2}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FB1E3C0E-653D-4DA7-A093-4271DA0134D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw_Data" sheetId="2" r:id="rId1"/>
@@ -39,19 +39,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
   <futureMetadata name="XLRICHVALUE" count="49">
     <bk>
       <extLst>
@@ -397,165 +387,160 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <cellMetadata count="1">
+  <valueMetadata count="49">
     <bk>
       <rc t="1" v="0"/>
     </bk>
-  </cellMetadata>
-  <valueMetadata count="49">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-    <bk>
-      <rc t="2" v="1"/>
-    </bk>
-    <bk>
-      <rc t="2" v="2"/>
-    </bk>
-    <bk>
-      <rc t="2" v="3"/>
-    </bk>
-    <bk>
-      <rc t="2" v="4"/>
-    </bk>
-    <bk>
-      <rc t="2" v="5"/>
-    </bk>
-    <bk>
-      <rc t="2" v="6"/>
-    </bk>
-    <bk>
-      <rc t="2" v="7"/>
-    </bk>
-    <bk>
-      <rc t="2" v="8"/>
-    </bk>
-    <bk>
-      <rc t="2" v="9"/>
-    </bk>
-    <bk>
-      <rc t="2" v="10"/>
-    </bk>
-    <bk>
-      <rc t="2" v="11"/>
-    </bk>
-    <bk>
-      <rc t="2" v="12"/>
-    </bk>
-    <bk>
-      <rc t="2" v="13"/>
-    </bk>
-    <bk>
-      <rc t="2" v="14"/>
-    </bk>
-    <bk>
-      <rc t="2" v="15"/>
-    </bk>
-    <bk>
-      <rc t="2" v="16"/>
-    </bk>
-    <bk>
-      <rc t="2" v="17"/>
-    </bk>
-    <bk>
-      <rc t="2" v="18"/>
-    </bk>
-    <bk>
-      <rc t="2" v="19"/>
-    </bk>
-    <bk>
-      <rc t="2" v="20"/>
-    </bk>
-    <bk>
-      <rc t="2" v="21"/>
-    </bk>
-    <bk>
-      <rc t="2" v="22"/>
-    </bk>
-    <bk>
-      <rc t="2" v="23"/>
-    </bk>
-    <bk>
-      <rc t="2" v="24"/>
-    </bk>
-    <bk>
-      <rc t="2" v="25"/>
-    </bk>
-    <bk>
-      <rc t="2" v="26"/>
-    </bk>
-    <bk>
-      <rc t="2" v="27"/>
-    </bk>
-    <bk>
-      <rc t="2" v="28"/>
-    </bk>
-    <bk>
-      <rc t="2" v="29"/>
-    </bk>
-    <bk>
-      <rc t="2" v="30"/>
-    </bk>
-    <bk>
-      <rc t="2" v="31"/>
-    </bk>
-    <bk>
-      <rc t="2" v="32"/>
-    </bk>
-    <bk>
-      <rc t="2" v="33"/>
-    </bk>
-    <bk>
-      <rc t="2" v="34"/>
-    </bk>
-    <bk>
-      <rc t="2" v="35"/>
-    </bk>
-    <bk>
-      <rc t="2" v="36"/>
-    </bk>
-    <bk>
-      <rc t="2" v="37"/>
-    </bk>
-    <bk>
-      <rc t="2" v="38"/>
-    </bk>
-    <bk>
-      <rc t="2" v="39"/>
-    </bk>
-    <bk>
-      <rc t="2" v="40"/>
-    </bk>
-    <bk>
-      <rc t="2" v="41"/>
-    </bk>
-    <bk>
-      <rc t="2" v="42"/>
-    </bk>
-    <bk>
-      <rc t="2" v="43"/>
-    </bk>
-    <bk>
-      <rc t="2" v="44"/>
-    </bk>
-    <bk>
-      <rc t="2" v="45"/>
-    </bk>
-    <bk>
-      <rc t="2" v="46"/>
-    </bk>
-    <bk>
-      <rc t="2" v="47"/>
-    </bk>
-    <bk>
-      <rc t="2" v="48"/>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+    <bk>
+      <rc t="1" v="14"/>
+    </bk>
+    <bk>
+      <rc t="1" v="15"/>
+    </bk>
+    <bk>
+      <rc t="1" v="16"/>
+    </bk>
+    <bk>
+      <rc t="1" v="17"/>
+    </bk>
+    <bk>
+      <rc t="1" v="18"/>
+    </bk>
+    <bk>
+      <rc t="1" v="19"/>
+    </bk>
+    <bk>
+      <rc t="1" v="20"/>
+    </bk>
+    <bk>
+      <rc t="1" v="21"/>
+    </bk>
+    <bk>
+      <rc t="1" v="22"/>
+    </bk>
+    <bk>
+      <rc t="1" v="23"/>
+    </bk>
+    <bk>
+      <rc t="1" v="24"/>
+    </bk>
+    <bk>
+      <rc t="1" v="25"/>
+    </bk>
+    <bk>
+      <rc t="1" v="26"/>
+    </bk>
+    <bk>
+      <rc t="1" v="27"/>
+    </bk>
+    <bk>
+      <rc t="1" v="28"/>
+    </bk>
+    <bk>
+      <rc t="1" v="29"/>
+    </bk>
+    <bk>
+      <rc t="1" v="30"/>
+    </bk>
+    <bk>
+      <rc t="1" v="31"/>
+    </bk>
+    <bk>
+      <rc t="1" v="32"/>
+    </bk>
+    <bk>
+      <rc t="1" v="33"/>
+    </bk>
+    <bk>
+      <rc t="1" v="34"/>
+    </bk>
+    <bk>
+      <rc t="1" v="35"/>
+    </bk>
+    <bk>
+      <rc t="1" v="36"/>
+    </bk>
+    <bk>
+      <rc t="1" v="37"/>
+    </bk>
+    <bk>
+      <rc t="1" v="38"/>
+    </bk>
+    <bk>
+      <rc t="1" v="39"/>
+    </bk>
+    <bk>
+      <rc t="1" v="40"/>
+    </bk>
+    <bk>
+      <rc t="1" v="41"/>
+    </bk>
+    <bk>
+      <rc t="1" v="42"/>
+    </bk>
+    <bk>
+      <rc t="1" v="43"/>
+    </bk>
+    <bk>
+      <rc t="1" v="44"/>
+    </bk>
+    <bk>
+      <rc t="1" v="45"/>
+    </bk>
+    <bk>
+      <rc t="1" v="46"/>
+    </bk>
+    <bk>
+      <rc t="1" v="47"/>
+    </bk>
+    <bk>
+      <rc t="1" v="48"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="147">
   <si>
     <t>Company</t>
   </si>
@@ -894,13 +879,115 @@
   </si>
   <si>
     <t>Change BRK.B for BRK-B</t>
+  </si>
+  <si>
+    <t>Industry from https://www.sec.gov/edgar/searchedgar/companysearch</t>
+  </si>
+  <si>
+    <t>Electronic Computers</t>
+  </si>
+  <si>
+    <t>Services-Prepackaged Software</t>
+  </si>
+  <si>
+    <t>Retail-Catalog &amp; Mail-Order Houses</t>
+  </si>
+  <si>
+    <t>Services-Computer Programming Data Processing Etc.</t>
+  </si>
+  <si>
+    <t>Fire Marine &amp; Casualty Insurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Semiconductors &amp; Related Devices</t>
+  </si>
+  <si>
+    <t>Motor Vehicles &amp; Passenger Car Bodies</t>
+  </si>
+  <si>
+    <t>Petroleum Refining</t>
+  </si>
+  <si>
+    <t>Hospital &amp; Medical Service Plans</t>
+  </si>
+  <si>
+    <t>Pharmaceutical Preparations</t>
+  </si>
+  <si>
+    <t> Services-Computer Programming Data Processing Etc.</t>
+  </si>
+  <si>
+    <t>National Commercial Banks</t>
+  </si>
+  <si>
+    <t>Services-Business Services NEC</t>
+  </si>
+  <si>
+    <t>Retail-Lumber &amp; Other Building Materials Dealers</t>
+  </si>
+  <si>
+    <t>Soap Detergents Cleang Preparations Perfumes Cosmetics</t>
+  </si>
+  <si>
+    <t>Semiconductors &amp; Related Devices</t>
+  </si>
+  <si>
+    <t>Beverages</t>
+  </si>
+  <si>
+    <t>Retail-Variety Stores</t>
+  </si>
+  <si>
+    <t>Measuring &amp; Controlling Devices NEC</t>
+  </si>
+  <si>
+    <t>NEC = Not elsewhere classified</t>
+  </si>
+  <si>
+    <t>Services-Miscellaneous Amusement &amp; Recreation</t>
+  </si>
+  <si>
+    <t>Retail-Eating Places</t>
+  </si>
+  <si>
+    <t>Computer Communications Equipment</t>
+  </si>
+  <si>
+    <t>Telephone Communications (No Radiotelephone)</t>
+  </si>
+  <si>
+    <t> Industrial Instruments For Measurement Display and Control</t>
+  </si>
+  <si>
+    <t>Cable &amp; Other Pay Television Services</t>
+  </si>
+  <si>
+    <t>Services-Video Tape Rental</t>
+  </si>
+  <si>
+    <t>Industrial Inorganic Chemicals</t>
+  </si>
+  <si>
+    <t>Rubber &amp; Plastics Footwear</t>
+  </si>
+  <si>
+    <t>Cigarettes</t>
+  </si>
+  <si>
+    <t>Electric Services</t>
+  </si>
+  <si>
+    <t>Radio &amp; Tv Broadcasting &amp; Communications Equipment</t>
+  </si>
+  <si>
+    <t>Aircraft Engines &amp; Engine Parts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -915,6 +1002,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -937,11 +1030,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4409,14 +4503,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4436,7 +4530,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4455,7 +4549,7 @@
         <v>6.5920629999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4474,7 +4568,7 @@
         <v>12.153207999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4493,7 +4587,7 @@
         <v>14.788079</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -4512,7 +4606,7 @@
         <v>16.573792000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -4531,7 +4625,7 @@
         <v>18.188330000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4550,7 +4644,7 @@
         <v>18.188330000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -4569,7 +4663,7 @@
         <v>19.715691</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -4588,7 +4682,7 @@
         <v>21.234493000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -4607,7 +4701,7 @@
         <v>22.571362000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -4626,7 +4720,7 @@
         <v>23.861466</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -4645,7 +4739,7 @@
         <v>25.103732000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -4664,7 +4758,7 @@
         <v>26.319310999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -4683,7 +4777,7 @@
         <v>27.528769</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -4702,7 +4796,7 @@
         <v>28.618687000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -4721,7 +4815,7 @@
         <v>29.597484000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -4740,7 +4834,7 @@
         <v>30.571009</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4759,7 +4853,7 @@
         <v>31.491388000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -4778,7 +4872,7 @@
         <v>32.368169999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -4797,7 +4891,7 @@
         <v>33.141869</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -4816,7 +4910,7 @@
         <v>33.908181999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -4835,7 +4929,7 @@
         <v>34.653313999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -4854,7 +4948,7 @@
         <v>35.390830999999991</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -4873,7 +4967,7 @@
         <v>36.104505999999994</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -4892,7 +4986,7 @@
         <v>36.812063999999992</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -4911,7 +5005,7 @@
         <v>37.499816999999993</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -4930,7 +5024,7 @@
         <v>38.18021499999999</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -4949,7 +5043,7 @@
         <v>38.84325299999999</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -4968,7 +5062,7 @@
         <v>39.499802999999993</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -4987,7 +5081,7 @@
         <v>40.081746999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -5006,7 +5100,7 @@
         <v>40.658626999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -5025,7 +5119,7 @@
         <v>41.228607999999994</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -5044,7 +5138,7 @@
         <v>41.796092999999992</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -5063,7 +5157,7 @@
         <v>42.356922999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -5082,7 +5176,7 @@
         <v>42.884786999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -5101,7 +5195,7 @@
         <v>43.404896999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -5120,7 +5214,7 @@
         <v>43.913330999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -5139,7 +5233,7 @@
         <v>44.417032999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -5158,7 +5252,7 @@
         <v>44.919078999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -5177,7 +5271,7 @@
         <v>45.414286999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -5196,7 +5290,7 @@
         <v>45.905442999999991</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -5215,7 +5309,7 @@
         <v>46.384309999999992</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -5234,7 +5328,7 @@
         <v>46.851682999999994</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -5253,7 +5347,7 @@
         <v>47.315433999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -5272,7 +5366,7 @@
         <v>47.775618999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -5291,7 +5385,7 @@
         <v>48.235593000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -5310,7 +5404,7 @@
         <v>48.694141000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -5329,7 +5423,7 @@
         <v>49.130099000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -5348,7 +5442,7 @@
         <v>49.562302000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -5367,7 +5461,7 @@
         <v>49.97972</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -5398,12 +5492,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5417,7 +5511,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5431,7 +5525,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -5442,7 +5536,7 @@
         <v>5.5611449999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5453,7 +5547,7 @@
         <v>2.634871</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -5464,7 +5558,7 @@
         <v>1.7857130000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -5475,7 +5569,7 @@
         <v>1.614538</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -5486,7 +5580,7 @@
         <v>1.527361</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -5497,7 +5591,7 @@
         <v>1.518802</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -5508,7 +5602,7 @@
         <v>1.3368690000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -5519,7 +5613,7 @@
         <v>1.2901039999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -5530,7 +5624,7 @@
         <v>1.2422660000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -5541,7 +5635,7 @@
         <v>1.215579</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -5552,7 +5646,7 @@
         <v>1.2094579999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -5563,7 +5657,7 @@
         <v>1.0899179999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -5574,7 +5668,7 @@
         <v>0.97879700000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -5585,7 +5679,7 @@
         <v>0.97352499999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -5596,7 +5690,7 @@
         <v>0.92037899999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -5607,7 +5701,7 @@
         <v>0.87678199999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -5618,7 +5712,7 @@
         <v>0.77369900000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -5629,7 +5723,7 @@
         <v>0.76631300000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -5640,7 +5734,7 @@
         <v>0.74513200000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -5651,7 +5745,7 @@
         <v>0.73751699999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -5662,7 +5756,7 @@
         <v>0.71367499999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -5673,7 +5767,7 @@
         <v>0.70755800000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -5684,7 +5778,7 @@
         <v>0.68775299999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -5695,7 +5789,7 @@
         <v>0.68039799999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -5706,7 +5800,7 @@
         <v>0.66303800000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -5717,7 +5811,7 @@
         <v>0.65654999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -5728,7 +5822,7 @@
         <v>0.58194400000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -5739,7 +5833,7 @@
         <v>0.57687999999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -5750,7 +5844,7 @@
         <v>0.56998099999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -5761,7 +5855,7 @@
         <v>0.56748500000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -5772,7 +5866,7 @@
         <v>0.56083000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -5783,7 +5877,7 @@
         <v>0.527864</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -5794,7 +5888,7 @@
         <v>0.52010999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -5805,7 +5899,7 @@
         <v>0.50843400000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -5816,7 +5910,7 @@
         <v>0.50370199999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -5827,7 +5921,7 @@
         <v>0.50204599999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -5838,7 +5932,7 @@
         <v>0.49520799999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -5849,7 +5943,7 @@
         <v>0.49115599999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -5860,7 +5954,7 @@
         <v>0.47886699999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -5871,7 +5965,7 @@
         <v>0.46737299999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -5882,7 +5976,7 @@
         <v>0.46375100000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -5893,7 +5987,7 @@
         <v>0.46018500000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -5904,7 +5998,7 @@
         <v>0.45997399999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -5915,7 +6009,7 @@
         <v>0.45854800000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -5926,7 +6020,7 @@
         <v>0.43595800000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -5937,7 +6031,7 @@
         <v>0.432203</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -5948,7 +6042,7 @@
         <v>0.41741800000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -5972,17 +6066,15 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="48.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5996,597 +6088,553 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" t="str" cm="1">
-        <f t="array" ref="C2">_FV(B2,"Industry")</f>
-        <v>Computers, Phones &amp; Household Electronics</v>
+      <c r="C2" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="C3" t="str" cm="1">
-        <f t="array" ref="C3">_FV(B3,"Industry")</f>
-        <v>Software &amp; IT Services</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="C4" t="str" cm="1">
-        <f t="array" ref="C4">_FV(B4,"Industry")</f>
-        <v>Diversified Retail</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
-      <c r="C5" t="str" cm="1">
-        <f t="array" ref="C5">_FV(B5,"Industry")</f>
-        <v>Software &amp; IT Services</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>110</v>
       </c>
       <c r="B6" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="C6" t="str" cm="1">
-        <f t="array" ref="C6">_FV(B6,"Industry")</f>
-        <v>Consumer Goods Conglomerates</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
-      <c r="C7" t="str" cm="1">
-        <f t="array" ref="C7">_FV(B7,"Industry")</f>
-        <v>Semiconductors &amp; Semiconductor Equipment</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
-      <c r="C8" t="str" cm="1">
-        <f t="array" ref="C8">_FV(B8,"Industry")</f>
-        <v>Automobiles &amp; Auto Parts</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
-      <c r="C9" t="str" cm="1">
-        <f t="array" ref="C9">_FV(B9,"Industry")</f>
-        <v>Oil &amp; Gas</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
-      <c r="C10" t="str" cm="1">
-        <f t="array" ref="C10">_FV(B10,"Industry")</f>
-        <v>Healthcare Providers &amp; Services</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
-      <c r="C11" t="str" cm="1">
-        <f t="array" ref="C11">_FV(B11,"Industry")</f>
-        <v>Pharmaceuticals</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
-      <c r="C12" t="str" cm="1">
-        <f t="array" ref="C12">_FV(B12,"Industry")</f>
-        <v>Software &amp; IT Services</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
-      <c r="C13" t="str" cm="1">
-        <f t="array" ref="C13">_FV(B13,"Industry")</f>
-        <v>Banking Services</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
-      <c r="C14" t="str" cm="1">
-        <f t="array" ref="C14">_FV(B14,"Industry")</f>
-        <v>Software &amp; IT Services</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
-      <c r="C15" t="str" cm="1">
-        <f t="array" ref="C15">_FV(B15,"Industry")</f>
-        <v>Specialty Retailers</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
-      <c r="C16" t="str" cm="1">
-        <f t="array" ref="C16">_FV(B16,"Industry")</f>
-        <v>Personal &amp; Household Products &amp; Services</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
-      <c r="C17" t="str" cm="1">
-        <f t="array" ref="C17">_FV(B17,"Industry")</f>
-        <v>Software &amp; IT Services</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
       <c r="B18" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
-      <c r="C18" t="str" cm="1">
-        <f t="array" ref="C18">_FV(B18,"Industry")</f>
-        <v>Oil &amp; Gas</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>40</v>
       </c>
       <c r="B19" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
-      <c r="C19" t="str" cm="1">
-        <f t="array" ref="C19">_FV(B19,"Industry")</f>
-        <v>Pharmaceuticals</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
       <c r="B20" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
-      <c r="C20" t="str" cm="1">
-        <f t="array" ref="C20">_FV(B20,"Industry")</f>
-        <v>Pharmaceuticals</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
       <c r="B21" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
-      <c r="C21" t="str" cm="1">
-        <f t="array" ref="C21">_FV(B21,"Industry")</f>
-        <v>Pharmaceuticals</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
       <c r="B22" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
-      <c r="C22" t="str" cm="1">
-        <f t="array" ref="C22">_FV(B22,"Industry")</f>
-        <v>Banking Services</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
-      <c r="C23" t="str" cm="1">
-        <f t="array" ref="C23">_FV(B23,"Industry")</f>
-        <v>Pharmaceuticals</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C23" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="B24" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
-      <c r="C24" t="str" cm="1">
-        <f t="array" ref="C24">_FV(B24,"Industry")</f>
-        <v>Semiconductors &amp; Semiconductor Equipment</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>52</v>
       </c>
       <c r="B25" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
-      <c r="C25" t="str" cm="1">
-        <f t="array" ref="C25">_FV(B25,"Industry")</f>
-        <v>Beverages</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>54</v>
       </c>
       <c r="B26" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
-      <c r="C26" t="str" cm="1">
-        <f t="array" ref="C26">_FV(B26,"Industry")</f>
-        <v>Beverages</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>56</v>
       </c>
       <c r="B27" t="e" vm="26">
         <v>#VALUE!</v>
       </c>
-      <c r="C27" t="str" cm="1">
-        <f t="array" ref="C27">_FV(B27,"Industry")</f>
-        <v>Diversified Retail</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>58</v>
       </c>
       <c r="B28" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
-      <c r="C28" t="str" cm="1">
-        <f t="array" ref="C28">_FV(B28,"Industry")</f>
-        <v>Healthcare Equipment &amp; Supplies</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>60</v>
       </c>
       <c r="B29" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
-      <c r="C29" t="str" cm="1">
-        <f t="array" ref="C29">_FV(B29,"Industry")</f>
-        <v>Media &amp; Publishing</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>62</v>
       </c>
       <c r="B30" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
-      <c r="C30" t="str" cm="1">
-        <f t="array" ref="C30">_FV(B30,"Industry")</f>
-        <v>Food &amp; Drug Retailing</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>64</v>
       </c>
       <c r="B31" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
-      <c r="C31" t="str" cm="1">
-        <f t="array" ref="C31">_FV(B31,"Industry")</f>
-        <v>Hotels &amp; Entertainment Services</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>66</v>
       </c>
       <c r="B32" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
-      <c r="C32" t="str" cm="1">
-        <f t="array" ref="C32">_FV(B32,"Industry")</f>
-        <v>Communications &amp; Networking</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C32" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>68</v>
       </c>
       <c r="B33" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
-      <c r="C33" t="str" cm="1">
-        <f t="array" ref="C33">_FV(B33,"Industry")</f>
-        <v>Healthcare Equipment &amp; Supplies</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>70</v>
       </c>
       <c r="B34" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
-      <c r="C34" t="str" cm="1">
-        <f t="array" ref="C34">_FV(B34,"Industry")</f>
-        <v>Banking Services</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>72</v>
       </c>
       <c r="B35" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
-      <c r="C35" t="str" cm="1">
-        <f t="array" ref="C35">_FV(B35,"Industry")</f>
-        <v>Software &amp; IT Services</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>74</v>
       </c>
       <c r="B36" t="e" vm="35">
         <v>#VALUE!</v>
       </c>
-      <c r="C36" t="str" cm="1">
-        <f t="array" ref="C36">_FV(B36,"Industry")</f>
-        <v>Software &amp; IT Services</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>76</v>
       </c>
       <c r="B37" t="e" vm="36">
         <v>#VALUE!</v>
       </c>
-      <c r="C37" t="str" cm="1">
-        <f t="array" ref="C37">_FV(B37,"Industry")</f>
-        <v>Telecommunications Services</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>78</v>
       </c>
       <c r="B38" t="e" vm="37">
         <v>#VALUE!</v>
       </c>
-      <c r="C38" t="str" cm="1">
-        <f t="array" ref="C38">_FV(B38,"Industry")</f>
-        <v>Healthcare Equipment &amp; Supplies</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>80</v>
       </c>
       <c r="B39" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
-      <c r="C39" t="str" cm="1">
-        <f t="array" ref="C39">_FV(B39,"Industry")</f>
-        <v>Telecommunications Services</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>82</v>
       </c>
       <c r="B40" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
-      <c r="C40" t="str" cm="1">
-        <f t="array" ref="C40">_FV(B40,"Industry")</f>
-        <v>Software &amp; IT Services</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>84</v>
       </c>
       <c r="B41" t="e" vm="40">
         <v>#VALUE!</v>
       </c>
-      <c r="C41" t="str" cm="1">
-        <f t="array" ref="C41">_FV(B41,"Industry")</f>
-        <v>Semiconductors &amp; Semiconductor Equipment</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>86</v>
       </c>
       <c r="B42" t="e" vm="41">
         <v>#VALUE!</v>
       </c>
-      <c r="C42" t="str" cm="1">
-        <f t="array" ref="C42">_FV(B42,"Industry")</f>
-        <v>Software &amp; IT Services</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>88</v>
       </c>
       <c r="B43" t="e" vm="42">
         <v>#VALUE!</v>
       </c>
-      <c r="C43" t="str" cm="1">
-        <f t="array" ref="C43">_FV(B43,"Industry")</f>
-        <v>Chemicals</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>90</v>
       </c>
       <c r="B44" t="e" vm="43">
         <v>#VALUE!</v>
       </c>
-      <c r="C44" t="str" cm="1">
-        <f t="array" ref="C44">_FV(B44,"Industry")</f>
-        <v>Pharmaceuticals</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>92</v>
       </c>
       <c r="B45" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
-      <c r="C45" t="str" cm="1">
-        <f t="array" ref="C45">_FV(B45,"Industry")</f>
-        <v>Textiles &amp; Apparel</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>94</v>
       </c>
       <c r="B46" t="e" vm="45">
         <v>#VALUE!</v>
       </c>
-      <c r="C46" t="str" cm="1">
-        <f t="array" ref="C46">_FV(B46,"Industry")</f>
-        <v>Food &amp; Tobacco</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>96</v>
       </c>
       <c r="B47" t="e" vm="46">
         <v>#VALUE!</v>
       </c>
-      <c r="C47" t="str" cm="1">
-        <f t="array" ref="C47">_FV(B47,"Industry")</f>
-        <v>Electrical Utilities &amp; IPPs</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C47" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>98</v>
       </c>
       <c r="B48" t="e" vm="47">
         <v>#VALUE!</v>
       </c>
-      <c r="C48" t="str" cm="1">
-        <f t="array" ref="C48">_FV(B48,"Industry")</f>
-        <v>Semiconductors &amp; Semiconductor Equipment</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>100</v>
       </c>
       <c r="B49" t="e" vm="48">
         <v>#VALUE!</v>
       </c>
-      <c r="C49" t="str" cm="1">
-        <f t="array" ref="C49">_FV(B49,"Industry")</f>
-        <v>Aerospace &amp; Defense</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>102</v>
       </c>
       <c r="B50" t="e" vm="49">
         <v>#VALUE!</v>
       </c>
-      <c r="C50" t="str" cm="1">
-        <f t="array" ref="C50">_FV(B50,"Industry")</f>
-        <v>Telecommunications Services</v>
+      <c r="C50" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>